<commit_message>
Updated whatsapp for 2024.2, added test data
</commit_message>
<xml_diff>
--- a/data/PS 2024.2 - Inscrição.xlsx
+++ b/data/PS 2024.2 - Inscrição.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28019"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gvmail.sharepoint.com/sites/GVCode/Documentos Compartilhados/Áreas/Processo Seletivo/2024.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="641" documentId="13_ncr:1_{B69B1C11-5624-405C-A33B-F0D19CDB1A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA250EAA-CA2B-4B99-BFEC-34E8CB46B76F}"/>
+  <xr:revisionPtr revIDLastSave="665" documentId="13_ncr:1_{B69B1C11-5624-405C-A33B-F0D19CDB1A74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F579CE08-6154-40C2-86FC-DAFB489B6CF2}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="915" windowWidth="21840" windowHeight="13140" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="915" windowWidth="21840" windowHeight="13140" firstSheet="3" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -89,13 +89,535 @@
     <t>Hora da última modificação</t>
   </si>
   <si>
+    <t>Nome completo:</t>
+  </si>
+  <si>
+    <t>Carteira</t>
+  </si>
+  <si>
+    <t>Celular</t>
+  </si>
+  <si>
+    <t>E-mail para contato:</t>
+  </si>
+  <si>
+    <t>Qual seu curso?</t>
+  </si>
+  <si>
+    <t>Semestre</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Nascimento</t>
+  </si>
+  <si>
+    <t>OndeConheceu</t>
+  </si>
+  <si>
+    <t>Dia1</t>
+  </si>
+  <si>
+    <t>Dia2</t>
+  </si>
+  <si>
+    <t>Dia3</t>
+  </si>
+  <si>
+    <t>Dia4</t>
+  </si>
+  <si>
+    <t>Dia5</t>
+  </si>
+  <si>
+    <t>C353595@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>RICARDO CASTRO</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Administração de Empresas</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Feminino</t>
+  </si>
+  <si>
+    <t>Professores;</t>
+  </si>
+  <si>
+    <t>9h - 10h30;</t>
+  </si>
+  <si>
+    <t>C375100@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>CAIO OLIVEIRA</t>
+  </si>
+  <si>
+    <t>Bruna Naomi Kita</t>
+  </si>
+  <si>
+    <t>C376994</t>
+  </si>
+  <si>
+    <t>brunakitaa@gmail.com</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Colegas;</t>
+  </si>
+  <si>
+    <t>Nenhum;</t>
+  </si>
+  <si>
+    <t>11h - 12h30;</t>
+  </si>
+  <si>
+    <t>15h - 16h30;</t>
+  </si>
+  <si>
+    <t>C371398@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>JÉSSICA SOUSA</t>
+  </si>
+  <si>
+    <t>Jessica Teixeira Sousa</t>
+  </si>
+  <si>
+    <t>C371398</t>
+  </si>
+  <si>
+    <t>(11)991695889</t>
+  </si>
+  <si>
+    <t>jessica.tsousa@gmail.com</t>
+  </si>
+  <si>
+    <t>3o</t>
+  </si>
+  <si>
+    <t>Instagram;</t>
+  </si>
+  <si>
+    <t>9h - 10h30;11h - 12h30;</t>
+  </si>
+  <si>
+    <t>19h - 20h30;</t>
+  </si>
+  <si>
+    <t>C373821@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>WIVIANE ZHENG</t>
+  </si>
+  <si>
+    <t>Wiviane zheng</t>
+  </si>
+  <si>
+    <t>C373821</t>
+  </si>
+  <si>
+    <t>19983393636</t>
+  </si>
+  <si>
+    <t>Wivizheng@gmail.com</t>
+  </si>
+  <si>
+    <t>Economia</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>C375022@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>PEDRO LIMA</t>
+  </si>
+  <si>
+    <t>Pedro Henrique Barbosa de Lima</t>
+  </si>
+  <si>
+    <t>C375022</t>
+  </si>
+  <si>
+    <t>(19) 981114751</t>
+  </si>
+  <si>
+    <t>phbl1404@gmail.com</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Feira de entidades;</t>
+  </si>
+  <si>
+    <t>C375523@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>GUILHERME BEIRÃO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guilherme de Aguiar Beirão </t>
+  </si>
+  <si>
+    <t>C375523</t>
+  </si>
+  <si>
+    <t>(11)99263-1438</t>
+  </si>
+  <si>
+    <t>guilhermenorio2017@outlook.com</t>
+  </si>
+  <si>
+    <t>Administração Pública</t>
+  </si>
+  <si>
+    <t>Colegas;Apresentação em sala;Instagram;Feira de entidades;</t>
+  </si>
+  <si>
+    <t>C379806@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>GUSTAVO TELES</t>
+  </si>
+  <si>
+    <t>Gustavo Soares Teles</t>
+  </si>
+  <si>
+    <t>C379806</t>
+  </si>
+  <si>
+    <t>11992794879</t>
+  </si>
+  <si>
+    <t>gustavo.soaresteles.ismart@gmail.com</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>17h - 18h30;</t>
+  </si>
+  <si>
+    <t>C370015@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>LEONARDO HAZAN</t>
+  </si>
+  <si>
+    <t>Leonardo Futuro Rodrigues Hazan</t>
+  </si>
+  <si>
+    <t>C370015</t>
+  </si>
+  <si>
+    <t>13996611828</t>
+  </si>
+  <si>
+    <t>leohazan@hotmail.com</t>
+  </si>
+  <si>
+    <t>5º</t>
+  </si>
+  <si>
+    <t>Feira de entidades;Postagem no grupo geral da gv adm de empresas;</t>
+  </si>
+  <si>
+    <t>15h - 16h30;17h - 18h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t>C379633@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>PEDRO ANTONIO</t>
+  </si>
+  <si>
+    <t>Pedro Henrique de Assis Marendaz Antonio</t>
+  </si>
+  <si>
+    <t>C379633</t>
+  </si>
+  <si>
+    <t>21999275717</t>
+  </si>
+  <si>
+    <t>phdeassisph@gmail.com</t>
+  </si>
+  <si>
+    <t>Colegas;Feira de entidades;</t>
+  </si>
+  <si>
+    <t>C373695@fgv.edu.br</t>
+  </si>
+  <si>
+    <t>FABRÍCIO WENTER</t>
+  </si>
+  <si>
+    <t>Fabrício Mello Wenter</t>
+  </si>
+  <si>
+    <t>C373695</t>
+  </si>
+  <si>
+    <t>11995004346</t>
+  </si>
+  <si>
+    <t>fabriciowenter88@gmail.com</t>
+  </si>
+  <si>
+    <t>Relações Internacionais</t>
+  </si>
+  <si>
+    <t>17h - 18h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t>15h - 16h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t>15h - 16h30;17h - 18h30;</t>
+  </si>
+  <si>
+    <t>anonymous</t>
+  </si>
+  <si>
+    <t>Luca Hora Ims Pires</t>
+  </si>
+  <si>
+    <t>C379686</t>
+  </si>
+  <si>
+    <t>79988373783</t>
+  </si>
+  <si>
+    <t>lucahora@gmail.com</t>
+  </si>
+  <si>
+    <t>17h - 18h30;15h - 16h30;</t>
+  </si>
+  <si>
+    <t>Ana Paula Menezes Dantas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B436247 (começa com B mesmo) </t>
+  </si>
+  <si>
+    <t>35 998030354</t>
+  </si>
+  <si>
+    <t>anapaulamdantas@gmail.com</t>
+  </si>
+  <si>
+    <t>17h - 18h30;13h - 14h30;</t>
+  </si>
+  <si>
+    <t>13h - 14h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t>Giovanna Vieira Izumi Garrido Farias</t>
+  </si>
+  <si>
+    <t>C373645</t>
+  </si>
+  <si>
+    <t>13981230121</t>
+  </si>
+  <si>
+    <t>gigi.izumi.farias@hotmail.com</t>
+  </si>
+  <si>
+    <t>Feira de entidades;Colegas;</t>
+  </si>
+  <si>
+    <t>13h - 14h30;15h - 16h30;</t>
+  </si>
+  <si>
+    <t>André Klinger Rocha</t>
+  </si>
+  <si>
+    <t>374766</t>
+  </si>
+  <si>
+    <t>11998731307</t>
+  </si>
+  <si>
+    <t>andre.k.rocha@icloud.com</t>
+  </si>
+  <si>
+    <t>4º</t>
+  </si>
+  <si>
+    <t>13h - 14h30;11h - 12h30;9h - 10h30;15h - 16h30;17h - 18h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t>9h - 10h30;11h - 12h30;13h - 14h30;15h - 16h30;17h - 18h30;19h - 20h30;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arthur Mendes Formiga </t>
+  </si>
+  <si>
+    <t>C374876</t>
+  </si>
+  <si>
+    <t>11991205912</t>
+  </si>
+  <si>
+    <t>formiga.arthur@gmail.com</t>
+  </si>
+  <si>
+    <t>Zicheng Hu</t>
+  </si>
+  <si>
+    <t>C376973</t>
+  </si>
+  <si>
+    <t>11983928180</t>
+  </si>
+  <si>
+    <t>woshitangyuanhu@gmail.com</t>
+  </si>
+  <si>
+    <t>13h - 14h30;15h - 16h30;17h - 18h30;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedro Morais </t>
+  </si>
+  <si>
+    <t>C374276</t>
+  </si>
+  <si>
+    <t>11996004610</t>
+  </si>
+  <si>
+    <t>Pedrohhm@outlook.com</t>
+  </si>
+  <si>
     <t>NomeCompleto</t>
   </si>
   <si>
-    <t>Carteira</t>
-  </si>
-  <si>
-    <t>Celular</t>
+    <t>Horário</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>_UIRAKzC002IjC7F3CaQQfPO31JPBRZLnBrBdwvxRN5UMVlaMjhLNVUxMFFIVTBRVjhYWTBVUFgzWCQlQCN0PWcu</t>
+  </si>
+  <si>
+    <t>Form1</t>
+  </si>
+  <si>
+    <t>{4dc27c40-7702-4d16-bb79-a604880331cf}</t>
+  </si>
+  <si>
+    <t>DinâmicaStatus</t>
+  </si>
+  <si>
+    <t>CaseStatus</t>
+  </si>
+  <si>
+    <t>EntrevistaStatus</t>
+  </si>
+  <si>
+    <t>DinâmicaNota</t>
+  </si>
+  <si>
+    <t>Case Nota</t>
+  </si>
+  <si>
+    <t>Entrevista Nota</t>
+  </si>
+  <si>
+    <t>[fazer um procv na planilha de case]</t>
+  </si>
+  <si>
+    <t>[fazer um procv na planilha de entrevista]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q1 </t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Pesos:</t>
+  </si>
+  <si>
+    <t>Nota máxima:</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>Valores padrões:</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Reprovado</t>
+  </si>
+  <si>
+    <t>Aprovado</t>
+  </si>
+  <si>
+    <t>Nomes das colunas:</t>
+  </si>
+  <si>
+    <t>Carteirinha</t>
   </si>
   <si>
     <t>EmailContato</t>
@@ -104,235 +626,10 @@
     <t>Curso</t>
   </si>
   <si>
-    <t>Semestre</t>
-  </si>
-  <si>
-    <t>Genero</t>
-  </si>
-  <si>
-    <t>Nascimento</t>
-  </si>
-  <si>
-    <t>OndeConheceu</t>
-  </si>
-  <si>
-    <t>Dia1</t>
-  </si>
-  <si>
-    <t>Dia2</t>
-  </si>
-  <si>
-    <t>Dia3</t>
-  </si>
-  <si>
-    <t>Dia4</t>
-  </si>
-  <si>
-    <t>Dia5</t>
-  </si>
-  <si>
-    <t>C353595@fgv.edu.br</t>
-  </si>
-  <si>
-    <t>RICARDO CASTRO</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>Administração de Empresas</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Feminino</t>
-  </si>
-  <si>
-    <t>Professores;</t>
-  </si>
-  <si>
-    <t>9h - 10h30;</t>
-  </si>
-  <si>
-    <t>C375100@fgv.edu.br</t>
-  </si>
-  <si>
-    <t>CAIO OLIVEIRA</t>
-  </si>
-  <si>
-    <t>Bruna Naomi Kita</t>
-  </si>
-  <si>
-    <t>C376994</t>
-  </si>
-  <si>
-    <t>brunakitaa@gmail.com</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Colegas;</t>
-  </si>
-  <si>
-    <t>Nenhum;</t>
-  </si>
-  <si>
-    <t>11h - 12h30;</t>
-  </si>
-  <si>
-    <t>15h - 16h30;</t>
-  </si>
-  <si>
-    <t>C371398@fgv.edu.br</t>
-  </si>
-  <si>
-    <t>JÉSSICA SOUSA</t>
-  </si>
-  <si>
-    <t>Jessica Teixeira Sousa</t>
-  </si>
-  <si>
-    <t>C371398</t>
-  </si>
-  <si>
-    <t>(11)991695889</t>
-  </si>
-  <si>
-    <t>jessica.tsousa@gmail.com</t>
-  </si>
-  <si>
-    <t>3o</t>
-  </si>
-  <si>
-    <t>Instagram;</t>
-  </si>
-  <si>
-    <t>9h - 10h30;11h - 12h30;</t>
-  </si>
-  <si>
-    <t>19h - 20h30;</t>
-  </si>
-  <si>
-    <t>Horário</t>
-  </si>
-  <si>
-    <t>Grupo</t>
-  </si>
-  <si>
-    <t>_UIRAKzC002IjC7F3CaQQfPO31JPBRZLnBrBdwvxRN5UMVlaMjhLNVUxMFFIVTBRVjhYWTBVUFgzWCQlQCN0PWcu</t>
-  </si>
-  <si>
-    <t>Form1</t>
-  </si>
-  <si>
-    <t>{4dc27c40-7702-4d16-bb79-a604880331cf}</t>
-  </si>
-  <si>
-    <t>Reprovado</t>
-  </si>
-  <si>
-    <t>[fazer um procv na planilha de case]</t>
-  </si>
-  <si>
-    <t>[fazer um procv na planilha de entrevista]</t>
-  </si>
-  <si>
-    <t>Aprovado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q1 </t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>Q6</t>
-  </si>
-  <si>
-    <t>Q7</t>
-  </si>
-  <si>
-    <t>Nota</t>
-  </si>
-  <si>
-    <t>Pesos:</t>
-  </si>
-  <si>
-    <t>Nota máxima:</t>
-  </si>
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>C3</t>
-  </si>
-  <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>Valores padrões:</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t>Status:</t>
-  </si>
-  <si>
-    <t>Nomes das colunas:</t>
-  </si>
-  <si>
-    <t>Carteirinha</t>
-  </si>
-  <si>
     <t>Alocação:</t>
   </si>
   <si>
     <t>Quando há dinâmicas em um mesmo horário, deve-se separar os grupos com números. Normalmente, só temos uma dinâmica por horário, e a coluna "Grupos" tem o valor 1</t>
-  </si>
-  <si>
-    <t>DinâmicaNota</t>
-  </si>
-  <si>
-    <t>Case Nota</t>
-  </si>
-  <si>
-    <t>Entrevista Nota</t>
-  </si>
-  <si>
-    <t>DinâmicaStatus</t>
-  </si>
-  <si>
-    <t>CaseStatus</t>
-  </si>
-  <si>
-    <t>EntrevistaStatus</t>
   </si>
 </sst>
 </file>
@@ -343,7 +640,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -684,11 +981,11 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,13 +1085,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T6" totalsRowShown="0">
-  <autoFilter ref="A1:T6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:T20" totalsRowShown="0">
+  <autoFilter ref="A1:T20" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de início" dataDxfId="21"/>
@@ -802,11 +1095,11 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="19"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nome" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Hora da última modificação" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{1153E0D8-B216-43A4-8E05-3CE3A5553CA0}" name="NomeCompleto" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{1153E0D8-B216-43A4-8E05-3CE3A5553CA0}" name="Nome completo:" dataDxfId="16"/>
     <tableColumn id="7" xr3:uid="{359CE1A3-0376-40EB-B375-5ADAC8520A23}" name="Carteira" dataDxfId="15"/>
     <tableColumn id="14" xr3:uid="{6C5B6077-704F-45BB-8F92-B53C4451FCED}" name="Celular" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{3DD5398A-A792-4320-9F31-8E6B4E538FBE}" name="EmailContato" dataDxfId="13"/>
-    <tableColumn id="21" xr3:uid="{DCC7299A-95B1-4D01-AD8D-0BF9E2C0BD59}" name="Curso" dataDxfId="12"/>
+    <tableColumn id="17" xr3:uid="{3DD5398A-A792-4320-9F31-8E6B4E538FBE}" name="E-mail para contato:" dataDxfId="13"/>
+    <tableColumn id="21" xr3:uid="{DCC7299A-95B1-4D01-AD8D-0BF9E2C0BD59}" name="Qual seu curso?" dataDxfId="12"/>
     <tableColumn id="23" xr3:uid="{B1F3DDE8-D1C5-40A3-9438-D816C754B7B5}" name="Semestre" dataDxfId="11"/>
     <tableColumn id="24" xr3:uid="{48712077-A72C-4D3B-9FEF-FD742421EABD}" name="Genero" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{B2E30E07-1B66-4097-A473-4A82774CA5E6}" name="Nascimento" dataDxfId="9"/>
@@ -1024,21 +1317,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="6" width="19.81640625" customWidth="1"/>
-    <col min="7" max="13" width="22.1796875" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" style="4" customWidth="1"/>
-    <col min="15" max="20" width="22.1796875" customWidth="1"/>
+    <col min="1" max="6" width="19.77734375" customWidth="1"/>
+    <col min="7" max="13" width="22.21875" customWidth="1"/>
+    <col min="14" max="14" width="22.21875" style="4" customWidth="1"/>
+    <col min="15" max="20" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" ht="17.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1393,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:20" ht="17.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1118,7 +1411,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:20" ht="17.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1136,7 +1429,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:20" ht="18.75" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1196,7 +1489,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:20" ht="18.75" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1256,7 +1549,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:20" ht="18.75" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1316,8 +1609,818 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I11" s="6"/>
+    <row r="7" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45524.792916666665</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45524.793865740743</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" t="s">
+        <v>34</v>
+      </c>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>35</v>
+      </c>
+      <c r="R7" t="s">
+        <v>35</v>
+      </c>
+      <c r="S7" t="s">
+        <v>35</v>
+      </c>
+      <c r="T7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45524.843622685185</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45524.846122685187</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="4">
+        <v>37360</v>
+      </c>
+      <c r="O8" t="s">
+        <v>63</v>
+      </c>
+      <c r="P8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>47</v>
+      </c>
+      <c r="R8" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45525.474027777775</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45525.485127314816</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="4">
+        <v>37613</v>
+      </c>
+      <c r="O9" t="s">
+        <v>71</v>
+      </c>
+      <c r="P9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>47</v>
+      </c>
+      <c r="R9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S9" t="s">
+        <v>47</v>
+      </c>
+      <c r="T9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45525.493622685186</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45525.495833333334</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" s="4">
+        <v>38530</v>
+      </c>
+      <c r="O10" t="s">
+        <v>63</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>47</v>
+      </c>
+      <c r="R10" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>45525.57503472222</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45525.582453703704</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11" t="s">
+        <v>85</v>
+      </c>
+      <c r="K11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="M11" t="s">
+        <v>62</v>
+      </c>
+      <c r="N11" s="4">
+        <v>36876</v>
+      </c>
+      <c r="O11" t="s">
+        <v>87</v>
+      </c>
+      <c r="P11" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" t="s">
+        <v>47</v>
+      </c>
+      <c r="S11" t="s">
+        <v>37</v>
+      </c>
+      <c r="T11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45525.599849537037</v>
+      </c>
+      <c r="C12" s="1">
+        <v>45525.614849537036</v>
+      </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J12" t="s">
+        <v>94</v>
+      </c>
+      <c r="K12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M12" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="4">
+        <v>38282</v>
+      </c>
+      <c r="O12" t="s">
+        <v>95</v>
+      </c>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>35</v>
+      </c>
+      <c r="R12" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" t="s">
+        <v>79</v>
+      </c>
+      <c r="T12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45525.700312499997</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45525.703599537039</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" t="s">
+        <v>102</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" t="s">
+        <v>62</v>
+      </c>
+      <c r="N13" s="4">
+        <v>38216</v>
+      </c>
+      <c r="O13" t="s">
+        <v>95</v>
+      </c>
+      <c r="P13" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>37</v>
+      </c>
+      <c r="R13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S13" t="s">
+        <v>105</v>
+      </c>
+      <c r="T13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45525.854097222225</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45525.855775462966</v>
+      </c>
+      <c r="D14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" t="s">
+        <v>62</v>
+      </c>
+      <c r="O14" t="s">
+        <v>45</v>
+      </c>
+      <c r="P14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>35</v>
+      </c>
+      <c r="R14" t="s">
+        <v>35</v>
+      </c>
+      <c r="S14" t="s">
+        <v>111</v>
+      </c>
+      <c r="T14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45525.935115740744</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45525.937824074077</v>
+      </c>
+      <c r="D15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="4">
+        <v>37712</v>
+      </c>
+      <c r="O15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>46</v>
+      </c>
+      <c r="R15" t="s">
+        <v>117</v>
+      </c>
+      <c r="S15" t="s">
+        <v>46</v>
+      </c>
+      <c r="T15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45525.90824074074</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45525.94158564815</v>
+      </c>
+      <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>119</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" t="s">
+        <v>102</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" t="s">
+        <v>122</v>
+      </c>
+      <c r="P16" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>35</v>
+      </c>
+      <c r="R16" t="s">
+        <v>35</v>
+      </c>
+      <c r="S16" t="s">
+        <v>123</v>
+      </c>
+      <c r="T16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45526.431620370371</v>
+      </c>
+      <c r="C17" s="1">
+        <v>45526.432534722226</v>
+      </c>
+      <c r="D17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J17" t="s">
+        <v>127</v>
+      </c>
+      <c r="K17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="M17" t="s">
+        <v>62</v>
+      </c>
+      <c r="N17" s="4">
+        <v>38181</v>
+      </c>
+      <c r="O17" t="s">
+        <v>63</v>
+      </c>
+      <c r="P17" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" t="s">
+        <v>35</v>
+      </c>
+      <c r="S17" t="s">
+        <v>129</v>
+      </c>
+      <c r="T17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45526.451423611114</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45526.454837962963</v>
+      </c>
+      <c r="D18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N18" s="4">
+        <v>38340</v>
+      </c>
+      <c r="O18" t="s">
+        <v>34</v>
+      </c>
+      <c r="P18" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" t="s">
+        <v>35</v>
+      </c>
+      <c r="S18" t="s">
+        <v>35</v>
+      </c>
+      <c r="T18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45526.567997685182</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45526.573391203703</v>
+      </c>
+      <c r="D19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
+      <c r="K19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M19" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="4">
+        <v>38116</v>
+      </c>
+      <c r="O19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>79</v>
+      </c>
+      <c r="R19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19" t="s">
+        <v>35</v>
+      </c>
+      <c r="T19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="18.75" customHeight="1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45526.715995370374</v>
+      </c>
+      <c r="C20" s="1">
+        <v>45526.719363425924</v>
+      </c>
+      <c r="D20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" t="s">
+        <v>143</v>
+      </c>
+      <c r="K20" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="4">
+        <v>38414</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>35</v>
+      </c>
+      <c r="R20" t="s">
+        <v>103</v>
+      </c>
+      <c r="S20" t="s">
+        <v>105</v>
+      </c>
+      <c r="T20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="18.75" customHeight="1">
+      <c r="I25" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1332,97 +2435,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FFF27B-830F-437B-9921-CA5C80823BC8}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" s="9" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="D2" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4">
       <c r="D3" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4">
       <c r="D4" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4">
       <c r="D5" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4">
       <c r="D6" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4">
       <c r="D7" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4">
       <c r="D8" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4">
       <c r="D9" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4">
       <c r="D10" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4">
       <c r="D11" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4">
       <c r="D12" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4">
       <c r="D13" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4">
       <c r="D14" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4">
       <c r="D15" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4">
       <c r="D16" s="10">
         <v>1</v>
       </c>
@@ -1438,21 +2541,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1465,56 +2568,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D3E7DC-0187-4283-AC9E-09FBAAA3703D}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" customHeight="1"/>
   <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8">
       <c r="A1" s="9" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>154</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="G2" t="s">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45"/>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8"/>
+    <row r="4" spans="1:8"/>
   </sheetData>
   <conditionalFormatting sqref="C1:E1048576">
     <cfRule type="expression" dxfId="2" priority="1">
@@ -1566,72 +2670,72 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.45"/>
   <cols>
-    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19">
       <c r="A1" s="9" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
       <c r="L1" s="11"/>
       <c r="M1" s="12" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>58</v>
+        <v>159</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="J2">
         <f t="shared" ref="J2:J14" si="0">SUMPRODUCT(C2:I2,$M$2:$S$2) / $M$3 * 5</f>
         <v>0</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="M2">
         <v>2</v>
@@ -1655,13 +2759,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19">
       <c r="J3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="M3" s="17" cm="1">
         <f t="array" ref="M3">SUM(5*(M2:S2))</f>
@@ -1674,67 +2778,67 @@
       <c r="R3" s="17"/>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19">
       <c r="J4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19">
       <c r="J5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19">
       <c r="J6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19">
       <c r="J7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19">
       <c r="J8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19">
       <c r="J9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19">
       <c r="J10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19">
       <c r="J11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19">
       <c r="J12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19">
       <c r="J13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19">
       <c r="J14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1753,72 +2857,72 @@
       <selection activeCell="L1" sqref="L1:S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.45"/>
   <cols>
-    <col min="12" max="12" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>67</v>
+        <v>168</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>64</v>
+        <v>165</v>
       </c>
       <c r="L1" s="11"/>
       <c r="M1" s="12" t="s">
-        <v>68</v>
+        <v>169</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>69</v>
+        <v>170</v>
       </c>
       <c r="O1" s="12" t="s">
-        <v>70</v>
+        <v>171</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>71</v>
+        <v>172</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>72</v>
+        <v>173</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>73</v>
+        <v>174</v>
       </c>
       <c r="S1" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="J2">
         <f t="shared" ref="J2:J14" si="0">SUMPRODUCT(C2:I2,$M$2:$S$2) / $M$3 * 5</f>
         <v>0</v>
       </c>
       <c r="L2" s="14" t="s">
-        <v>65</v>
+        <v>166</v>
       </c>
       <c r="M2">
         <v>3</v>
@@ -1842,13 +2946,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19">
       <c r="J3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>66</v>
+        <v>167</v>
       </c>
       <c r="M3" s="17" cm="1">
         <f t="array" ref="M3">SUM(5*(M2:S2))</f>
@@ -1861,67 +2965,67 @@
       <c r="R3" s="17"/>
       <c r="S3" s="18"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19">
       <c r="J4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19">
       <c r="J5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19">
       <c r="J6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19">
       <c r="J7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19">
       <c r="J8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19">
       <c r="J9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19">
       <c r="J10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19">
       <c r="J11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19">
       <c r="J12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19">
       <c r="J13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19">
       <c r="J14">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1940,24 +3044,24 @@
       <selection activeCell="F2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.45"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15">
       <c r="A1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="34"/>
+        <v>176</v>
+      </c>
+      <c r="B1" s="31"/>
       <c r="C1" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -1969,22 +3073,22 @@
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15">
       <c r="A2" s="22" t="s">
-        <v>77</v>
+        <v>178</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>53</v>
+        <v>179</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="35"/>
+        <v>180</v>
+      </c>
+      <c r="D2" s="32"/>
       <c r="E2" s="23" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -1996,7 +3100,7 @@
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="10"/>
@@ -2013,64 +3117,64 @@
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15">
       <c r="A4" s="25" t="s">
-        <v>78</v>
+        <v>181</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="G4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="I4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="J4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="N4" s="27" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="O4" s="10"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15">
       <c r="A5" s="28" t="s">
-        <v>6</v>
+        <v>144</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="C5" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>9</v>
+        <v>183</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>11</v>
@@ -2101,7 +3205,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -2118,71 +3222,71 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15">
       <c r="A7" s="19" t="s">
-        <v>80</v>
+        <v>185</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="J7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="33"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B8" s="34"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2193,26 +3297,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2807de7a-b882-44f5-9f07-3ac4d241cb3d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="18aaadd8-4fbe-433c-97a2-e75c8b57c8e6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001679527E1B0EA94E8138AA9ED30F4073" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="6866bf21d6896a2542552efefd485b9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2807de7a-b882-44f5-9f07-3ac4d241cb3d" xmlns:ns3="18aaadd8-4fbe-433c-97a2-e75c8b57c8e6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c6aa3b7f1cd58eea80c09626b94b3ae7" ns2:_="" ns3:_="">
     <xsd:import namespace="2807de7a-b882-44f5-9f07-3ac4d241cb3d"/>
@@ -2441,46 +3525,34 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="2807de7a-b882-44f5-9f07-3ac4d241cb3d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="18aaadd8-4fbe-433c-97a2-e75c8b57c8e6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08381228-0E8E-4962-B853-8CFAEB2E24F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32C1796-AEBB-4E0A-B4EA-D886969C4068}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D1C78A3-0709-4552-9112-859CF4352F27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="2807de7a-b882-44f5-9f07-3ac4d241cb3d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="18aaadd8-4fbe-433c-97a2-e75c8b57c8e6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08381228-0E8E-4962-B853-8CFAEB2E24F3}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32C1796-AEBB-4E0A-B4EA-D886969C4068}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2807de7a-b882-44f5-9f07-3ac4d241cb3d"/>
-    <ds:schemaRef ds:uri="18aaadd8-4fbe-433c-97a2-e75c8b57c8e6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D1C78A3-0709-4552-9112-859CF4352F27}"/>
 </file>
</xml_diff>